<commit_message>
refactor: convert all excel data to text
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\rfm\workspace\projects\identwork-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BE9D0-4463-4C4E-9AAF-1B0E6DE66A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BD5F64-279B-4DFE-B564-E4270CFDBEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>matricula</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Rodrigo Meneses</t>
   </si>
   <si>
-    <t>1,122,233,334</t>
-  </si>
-  <si>
     <t>PICI</t>
   </si>
   <si>
@@ -70,10 +67,19 @@
     <t>Marta Regina</t>
   </si>
   <si>
-    <t>4,433,322,221</t>
-  </si>
-  <si>
     <t>BENFICA</t>
+  </si>
+  <si>
+    <t>4433322221</t>
+  </si>
+  <si>
+    <t>1122233334</t>
+  </si>
+  <si>
+    <t>21/02/2020</t>
+  </si>
+  <si>
+    <t>15/04/2020</t>
   </si>
 </sst>
 </file>
@@ -155,45 +161,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -504,210 +487,211 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>123321</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6">
-        <v>43772</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>789987</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>789987</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="6">
-        <v>44569</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>13</v>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="6"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="6"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="6"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>